<commit_message>
Added proposals 91 file
</commit_message>
<xml_diff>
--- a/core/import_data/resources/sectors.xlsx
+++ b/core/import_data/resources/sectors.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>subsector</t>
   </si>
@@ -53,13 +53,34 @@
   </si>
   <si>
     <t>FOA</t>
+  </si>
+  <si>
+    <t>Preparation of project proposal</t>
+  </si>
+  <si>
+    <t>KIP</t>
+  </si>
+  <si>
+    <t>Domestic/commercial</t>
+  </si>
+  <si>
+    <t>HCFC closure</t>
+  </si>
+  <si>
+    <t>PRO</t>
+  </si>
+  <si>
+    <t>Agency programme</t>
+  </si>
+  <si>
+    <t>Technical assistance/support</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -80,13 +101,28 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -95,18 +131,20 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -337,84 +375,112 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
+      <c r="C1" s="1"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>7</v>
+      <c r="A6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="4" t="s">
+      <c r="A7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>10</v>
+      <c r="A8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>13</v>
+      <c r="A9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>7</v>
+        <v>14</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="11" ht="15.75" customHeight="1"/>
-    <row r="12" ht="15.75" customHeight="1"/>
-    <row r="13" ht="15.75" customHeight="1"/>
-    <row r="14" ht="15.75" customHeight="1"/>
+    <row r="11" ht="15.75" customHeight="1">
+      <c r="A11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" ht="15.75" customHeight="1">
+      <c r="A12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" ht="15.75" customHeight="1">
+      <c r="A13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" ht="15.75" customHeight="1">
+      <c r="A14" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
     <row r="15" ht="15.75" customHeight="1"/>
     <row r="16" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
@@ -1267,6 +1333,136 @@
     <row r="864" ht="15.75" customHeight="1"/>
     <row r="865" ht="15.75" customHeight="1"/>
     <row r="866" ht="15.75" customHeight="1"/>
+    <row r="867" ht="15.75" customHeight="1"/>
+    <row r="868" ht="15.75" customHeight="1"/>
+    <row r="869" ht="15.75" customHeight="1"/>
+    <row r="870" ht="15.75" customHeight="1"/>
+    <row r="871" ht="15.75" customHeight="1"/>
+    <row r="872" ht="15.75" customHeight="1"/>
+    <row r="873" ht="15.75" customHeight="1"/>
+    <row r="874" ht="15.75" customHeight="1"/>
+    <row r="875" ht="15.75" customHeight="1"/>
+    <row r="876" ht="15.75" customHeight="1"/>
+    <row r="877" ht="15.75" customHeight="1"/>
+    <row r="878" ht="15.75" customHeight="1"/>
+    <row r="879" ht="15.75" customHeight="1"/>
+    <row r="880" ht="15.75" customHeight="1"/>
+    <row r="881" ht="15.75" customHeight="1"/>
+    <row r="882" ht="15.75" customHeight="1"/>
+    <row r="883" ht="15.75" customHeight="1"/>
+    <row r="884" ht="15.75" customHeight="1"/>
+    <row r="885" ht="15.75" customHeight="1"/>
+    <row r="886" ht="15.75" customHeight="1"/>
+    <row r="887" ht="15.75" customHeight="1"/>
+    <row r="888" ht="15.75" customHeight="1"/>
+    <row r="889" ht="15.75" customHeight="1"/>
+    <row r="890" ht="15.75" customHeight="1"/>
+    <row r="891" ht="15.75" customHeight="1"/>
+    <row r="892" ht="15.75" customHeight="1"/>
+    <row r="893" ht="15.75" customHeight="1"/>
+    <row r="894" ht="15.75" customHeight="1"/>
+    <row r="895" ht="15.75" customHeight="1"/>
+    <row r="896" ht="15.75" customHeight="1"/>
+    <row r="897" ht="15.75" customHeight="1"/>
+    <row r="898" ht="15.75" customHeight="1"/>
+    <row r="899" ht="15.75" customHeight="1"/>
+    <row r="900" ht="15.75" customHeight="1"/>
+    <row r="901" ht="15.75" customHeight="1"/>
+    <row r="902" ht="15.75" customHeight="1"/>
+    <row r="903" ht="15.75" customHeight="1"/>
+    <row r="904" ht="15.75" customHeight="1"/>
+    <row r="905" ht="15.75" customHeight="1"/>
+    <row r="906" ht="15.75" customHeight="1"/>
+    <row r="907" ht="15.75" customHeight="1"/>
+    <row r="908" ht="15.75" customHeight="1"/>
+    <row r="909" ht="15.75" customHeight="1"/>
+    <row r="910" ht="15.75" customHeight="1"/>
+    <row r="911" ht="15.75" customHeight="1"/>
+    <row r="912" ht="15.75" customHeight="1"/>
+    <row r="913" ht="15.75" customHeight="1"/>
+    <row r="914" ht="15.75" customHeight="1"/>
+    <row r="915" ht="15.75" customHeight="1"/>
+    <row r="916" ht="15.75" customHeight="1"/>
+    <row r="917" ht="15.75" customHeight="1"/>
+    <row r="918" ht="15.75" customHeight="1"/>
+    <row r="919" ht="15.75" customHeight="1"/>
+    <row r="920" ht="15.75" customHeight="1"/>
+    <row r="921" ht="15.75" customHeight="1"/>
+    <row r="922" ht="15.75" customHeight="1"/>
+    <row r="923" ht="15.75" customHeight="1"/>
+    <row r="924" ht="15.75" customHeight="1"/>
+    <row r="925" ht="15.75" customHeight="1"/>
+    <row r="926" ht="15.75" customHeight="1"/>
+    <row r="927" ht="15.75" customHeight="1"/>
+    <row r="928" ht="15.75" customHeight="1"/>
+    <row r="929" ht="15.75" customHeight="1"/>
+    <row r="930" ht="15.75" customHeight="1"/>
+    <row r="931" ht="15.75" customHeight="1"/>
+    <row r="932" ht="15.75" customHeight="1"/>
+    <row r="933" ht="15.75" customHeight="1"/>
+    <row r="934" ht="15.75" customHeight="1"/>
+    <row r="935" ht="15.75" customHeight="1"/>
+    <row r="936" ht="15.75" customHeight="1"/>
+    <row r="937" ht="15.75" customHeight="1"/>
+    <row r="938" ht="15.75" customHeight="1"/>
+    <row r="939" ht="15.75" customHeight="1"/>
+    <row r="940" ht="15.75" customHeight="1"/>
+    <row r="941" ht="15.75" customHeight="1"/>
+    <row r="942" ht="15.75" customHeight="1"/>
+    <row r="943" ht="15.75" customHeight="1"/>
+    <row r="944" ht="15.75" customHeight="1"/>
+    <row r="945" ht="15.75" customHeight="1"/>
+    <row r="946" ht="15.75" customHeight="1"/>
+    <row r="947" ht="15.75" customHeight="1"/>
+    <row r="948" ht="15.75" customHeight="1"/>
+    <row r="949" ht="15.75" customHeight="1"/>
+    <row r="950" ht="15.75" customHeight="1"/>
+    <row r="951" ht="15.75" customHeight="1"/>
+    <row r="952" ht="15.75" customHeight="1"/>
+    <row r="953" ht="15.75" customHeight="1"/>
+    <row r="954" ht="15.75" customHeight="1"/>
+    <row r="955" ht="15.75" customHeight="1"/>
+    <row r="956" ht="15.75" customHeight="1"/>
+    <row r="957" ht="15.75" customHeight="1"/>
+    <row r="958" ht="15.75" customHeight="1"/>
+    <row r="959" ht="15.75" customHeight="1"/>
+    <row r="960" ht="15.75" customHeight="1"/>
+    <row r="961" ht="15.75" customHeight="1"/>
+    <row r="962" ht="15.75" customHeight="1"/>
+    <row r="963" ht="15.75" customHeight="1"/>
+    <row r="964" ht="15.75" customHeight="1"/>
+    <row r="965" ht="15.75" customHeight="1"/>
+    <row r="966" ht="15.75" customHeight="1"/>
+    <row r="967" ht="15.75" customHeight="1"/>
+    <row r="968" ht="15.75" customHeight="1"/>
+    <row r="969" ht="15.75" customHeight="1"/>
+    <row r="970" ht="15.75" customHeight="1"/>
+    <row r="971" ht="15.75" customHeight="1"/>
+    <row r="972" ht="15.75" customHeight="1"/>
+    <row r="973" ht="15.75" customHeight="1"/>
+    <row r="974" ht="15.75" customHeight="1"/>
+    <row r="975" ht="15.75" customHeight="1"/>
+    <row r="976" ht="15.75" customHeight="1"/>
+    <row r="977" ht="15.75" customHeight="1"/>
+    <row r="978" ht="15.75" customHeight="1"/>
+    <row r="979" ht="15.75" customHeight="1"/>
+    <row r="980" ht="15.75" customHeight="1"/>
+    <row r="981" ht="15.75" customHeight="1"/>
+    <row r="982" ht="15.75" customHeight="1"/>
+    <row r="983" ht="15.75" customHeight="1"/>
+    <row r="984" ht="15.75" customHeight="1"/>
+    <row r="985" ht="15.75" customHeight="1"/>
+    <row r="986" ht="15.75" customHeight="1"/>
+    <row r="987" ht="15.75" customHeight="1"/>
+    <row r="988" ht="15.75" customHeight="1"/>
+    <row r="989" ht="15.75" customHeight="1"/>
+    <row r="990" ht="15.75" customHeight="1"/>
+    <row r="991" ht="15.75" customHeight="1"/>
+    <row r="992" ht="15.75" customHeight="1"/>
+    <row r="993" ht="15.75" customHeight="1"/>
+    <row r="994" ht="15.75" customHeight="1"/>
+    <row r="995" ht="15.75" customHeight="1"/>
+    <row r="996" ht="15.75" customHeight="1"/>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>